<commit_message>
process-5 test the data and change
</commit_message>
<xml_diff>
--- a/data/process_05/inputData.xlsx
+++ b/data/process_05/inputData.xlsx
@@ -84,7 +84,7 @@
     <t>Custom Ref</t>
   </si>
   <si>
-    <t>Test5</t>
+    <t>Test10</t>
   </si>
 </sst>
 </file>
@@ -427,7 +427,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>

</xml_diff>